<commit_message>
B738 updated flow manual
</commit_message>
<xml_diff>
--- a/documentation/KPCrew Flows.xlsx
+++ b/documentation/KPCrew Flows.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="398">
   <si>
     <t xml:space="preserve">KPCREW FOR ZIBO BOEING 737-800 FREEWARE (V2.1x)</t>
   </si>
@@ -557,16 +557,30 @@
     <t xml:space="preserve">FLIGHT CONTROLS TEST</t>
   </si>
   <si>
-    <t xml:space="preserve">MOVE COLUMN FULL LEFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FULL LEFT – CTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOVE COLUMN FULL RIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FULL RIGHT – CTR</t>
+    <t xml:space="preserve">AILERON</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FULL LEFT – CTR – </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FULL RIGHT – CTR</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ELEVATORS</t>
@@ -593,79 +607,85 @@
     <t xml:space="preserve">ALTIMETERS</t>
   </si>
   <si>
+    <t xml:space="preserve">NAV AIDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET AND CHECKED</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISOLATION VALVES/PACKS</t>
   </si>
   <si>
-    <t xml:space="preserve">NAV AIDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET AND CHECKED</t>
-  </si>
-  <si>
     <t xml:space="preserve">HYDRAULICS</t>
   </si>
   <si>
     <t xml:space="preserve">ALL ON</t>
   </si>
   <si>
+    <t xml:space="preserve">LANDING PROCEDURE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENGINE START SWITCHES</t>
   </si>
   <si>
     <t xml:space="preserve">CONTINUOUS</t>
   </si>
   <si>
-    <t xml:space="preserve">LANDING PROCEDURE</t>
+    <t xml:space="preserve">LIGHTS</t>
   </si>
   <si>
     <t xml:space="preserve">APU</t>
   </si>
   <si>
-    <t xml:space="preserve">LIGHTS</t>
+    <t xml:space="preserve">AT 210 KTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAPS 1</t>
   </si>
   <si>
     <t xml:space="preserve">TAKEOFF FLAPS</t>
   </si>
   <si>
-    <t xml:space="preserve">AT 210 KTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLAPS 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">AT 180 KTS</t>
   </si>
   <si>
     <t xml:space="preserve">FLAPS 5</t>
   </si>
   <si>
+    <t xml:space="preserve">AT 160 KTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAPS 15 &amp; GEAR DOWN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEFORE TAXI CHECKLIST</t>
   </si>
   <si>
-    <t xml:space="preserve">AT 160 KTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLAPS 15 &amp; GEAR DOWN</t>
-  </si>
-  <si>
     <t xml:space="preserve">AT 155 KTS</t>
   </si>
   <si>
     <t xml:space="preserve">FLAPS 30</t>
   </si>
   <si>
+    <t xml:space="preserve">MISSED APPROACH ALTITUDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANTI-ICE</t>
   </si>
   <si>
-    <t xml:space="preserve">MISSED APPROACH ALTITUDE</t>
+    <t xml:space="preserve">LANDING CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">IDLE DETENT</t>
   </si>
   <si>
-    <t xml:space="preserve">LANDING CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">CABIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECURE</t>
   </si>
   <si>
     <t xml:space="preserve">FLIGHT CONTROLS </t>
@@ -674,12 +694,6 @@
     <t xml:space="preserve">CHECKED</t>
   </si>
   <si>
-    <t xml:space="preserve">CABIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECURE</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONT</t>
   </si>
   <si>
@@ -692,39 +706,39 @@
     <t xml:space="preserve">DOWN</t>
   </si>
   <si>
+    <t xml:space="preserve">FLAPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">___ GREEN LIGHT</t>
+  </si>
+  <si>
     <t xml:space="preserve">GROUND EQUIPMENT </t>
   </si>
   <si>
     <t xml:space="preserve">CLEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">FLAPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">___ GREEN LIGHT</t>
+    <t xml:space="preserve">FINAL PROCEDURE</t>
   </si>
   <si>
     <t xml:space="preserve">BEFORE TAKEOFF CHECKLIST</t>
   </si>
   <si>
-    <t xml:space="preserve">FINAL PROCEDURE</t>
+    <t xml:space="preserve">CLEARED FOR LANDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEARED</t>
   </si>
   <si>
     <t xml:space="preserve">FLAPS ___ , GREEN LIGHT</t>
   </si>
   <si>
-    <t xml:space="preserve">CLEARED FOR LANDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLEARED</t>
+    <t xml:space="preserve">AUTOPILOT</t>
   </si>
   <si>
     <t xml:space="preserve">___  POINT   ___  UNITS</t>
   </si>
   <si>
-    <t xml:space="preserve">AUTOPILOT</t>
-  </si>
-  <si>
     <t xml:space="preserve">TAKEOFF BRIEFING</t>
   </si>
   <si>
@@ -734,36 +748,36 @@
     <t xml:space="preserve">AFTER LANDING - CLEANUP</t>
   </si>
   <si>
+    <t xml:space="preserve">SPEEDBRAKES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UP</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEFORE TAKEOFF PROCEDURE                                 </t>
   </si>
   <si>
-    <t xml:space="preserve">SPEEDBRAKES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UP</t>
+    <t xml:space="preserve">CHRONO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP</t>
   </si>
   <si>
     <t xml:space="preserve">LANDING LIGHTS</t>
   </si>
   <si>
-    <t xml:space="preserve">CHRONO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STOP</t>
+    <t xml:space="preserve">WX RADAR (EFIS PANEL)</t>
   </si>
   <si>
     <t xml:space="preserve">STROBES</t>
   </si>
   <si>
-    <t xml:space="preserve">WX RADAR (EFIS PANEL)</t>
+    <t xml:space="preserve">START</t>
   </si>
   <si>
     <t xml:space="preserve">TAXI LIGHTS</t>
   </si>
   <si>
-    <t xml:space="preserve">START</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRANSPONDER</t>
   </si>
   <si>
@@ -785,37 +799,52 @@
     <t xml:space="preserve">TAKEOFF AND CLIMB PROCEDURE</t>
   </si>
   <si>
+    <t xml:space="preserve">TRAFFIC</t>
+  </si>
+  <si>
     <t xml:space="preserve">TAKEOFF THRUST</t>
   </si>
   <si>
-    <t xml:space="preserve">TRAFFIC</t>
-  </si>
-  <si>
     <t xml:space="preserve">HDG SEL</t>
   </si>
   <si>
+    <t xml:space="preserve">STANDBY</t>
+  </si>
+  <si>
     <t xml:space="preserve">EFIS WXR</t>
   </si>
   <si>
-    <t xml:space="preserve">STANDBY</t>
-  </si>
-  <si>
     <t xml:space="preserve">CALLOUTS</t>
   </si>
   <si>
+    <t xml:space="preserve">SHUTDOWN PROCEDURE</t>
+  </si>
+  <si>
     <t xml:space="preserve">GEAR</t>
   </si>
   <si>
-    <t xml:space="preserve">UP AND OFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHUTDOWN PROCEDURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A/P MODES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNAV/VNAV or HDG/FLCH</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UP AND OFF/</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MANUAL</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CMD A</t>
@@ -884,322 +913,340 @@
     <t xml:space="preserve">PACKS</t>
   </si>
   <si>
+    <t xml:space="preserve">UP AND OFF</t>
+  </si>
+  <si>
     <t xml:space="preserve">UP, NO LIGHTS</t>
   </si>
   <si>
     <t xml:space="preserve">ELAPSED TIME</t>
   </si>
   <si>
+    <t xml:space="preserve">SHUTDOWN CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPROACH BRIEFING – OPTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok, we will be arriving via &lt;ARRIVALTYPE&gt; &lt;ARRIVALNAME&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the arrival we can expect an &lt;TYPE&gt; approach into our destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UP NO LIGHTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runway assigned is &lt;RWY&gt; and the condition is &lt;CONDITION&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti Ice is &lt;ANTIICE SETTING&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landing flaps will be &lt;FLAPS&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEATHER RADAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for auto brake we will use level &lt;ABRKLVL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packs will be &lt;ON/OFF&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECURING AIRCRAFT PROCEDURE - OPTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision Height/Altitude will be &lt;HEIGHT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAB/UTIL &amp; IFE GALLEY POWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach speed &lt;SPD&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference speed &lt;SPD&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMERGENCY EXIT LIGHTS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missed approach altitude &gt;ALT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW HEAT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACKS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCENT CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESSURIZATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANDING ALTITUDE ___</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTERY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSITION LIGHT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">______</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANDING DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VREF ___, MINIMUMS ___ FEET*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECURE CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPROACH BRIEFING </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRSs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THROTTLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDLE FOR ZIBO DURING DESCENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPCREW FOR FLYJSIM B732 PAYWARE (V2.1x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TURN AROUND STATE – OPTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECT GPU IN MENU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APU START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GASPER FANS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAVIGATION PANEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEAT BELTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORMAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUEL QTY TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIR COND &amp; PRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK(S) SET, BLEEDS ON, SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTRUMENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-CHECKED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RADIOS, RADAR, TRANSPONDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OXYGEN &amp; INTERPHONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N1 &amp; IAS BUGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRELIMINARY FLIGHT COMPARTMENT CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OVERHEAT DETECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEARED FOR START PROCEDURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRE WARNING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISOLATION VLV OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTINGUISHER TEST SWITCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYDRAULIC PANEL SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARGO SMOKE/FIRE SYSTEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APU (IF REQUIRED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START/ON BUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERIFY TAKEOFF SPEEDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNOUNCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMERGENCY EQUIPMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIRCUIT BREAKERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLIGHT RECORDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEARED FOR START CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOBILE PHONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START PRESSURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASSENGER OXYGEN SWITCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTICOLLISION LIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GALLEY POWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIR CONDITIONING PACKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO SMOKING SIGNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTO PILOT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISENGAGED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTI-SKID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAP LEVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STABILIZER TRIM CUTOUT SWITCHES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHEEL WELL FIRE WARNING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIGHT TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREE &amp; ZERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAVIGATION TRANSFER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAPERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON BOARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMC/CDU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCENT APPROACH CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOVE COLUMN FULL LEFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FULL LEFT – CTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTI–ICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOVE COLUMN FULL RIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FULL RIGHT – CTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTIMETER &amp; INSTRUMENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET &amp; X-CHECKED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFTER START PROCEDURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFTER START CHECKLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELECTRICAL GENERATORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACKS ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLIGHT CONTROLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABIN DOOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANDING LIGHTS &amp; STROBES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A/P MODES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS/IAS or HDG/IAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELECTRICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON GPU/APU</t>
+  </si>
+  <si>
     <t xml:space="preserve">SET BOTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHUTDOWN CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPROACH BRIEFING – OPTIONAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ok, we will be arriving via &lt;ARRIVALTYPE&gt; &lt;ARRIVALNAME&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After the arrival we can expect an &lt;TYPE&gt; approach into our destination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UP NO LIGHTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runway assigned is &lt;RWY&gt; and the condition is &lt;CONDITION&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti Ice is &lt;ANTIICE SETTING&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Landing flaps will be &lt;FLAPS&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEATHER RADAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for auto brake we will use level &lt;ABRKLVL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packs will be &lt;ON/OFF&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECURING AIRCRAFT PROCEDURE - OPTIONAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision Height/Altitude will be &lt;HEIGHT&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAB/UTIL &amp; IFE GALLEY POWER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approach speed &lt;SPD&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference speed &lt;SPD&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMERGENCY EXIT LIGHTS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missed approach altitude &gt;ALT&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WINDOW HEAT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACKS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCENT CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APU </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRESSURIZATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LANDING ALTITUDE ___</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BATTERY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSITION LIGHT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">______</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LANDING DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VREF ___, MINIMUMS ___ FEET*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECURE CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPROACH BRIEFING </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRSs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THROTTLES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDLE FOR ZIBO DURING DESCENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPCREW FOR FLYJSIM B732 PAYWARE (V2.1x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TURN AROUND STATE – OPTIONAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONNECT GPU IN MENU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APU START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GASPER FANS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAVIGATION PANEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEAT BELTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NORMAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUEL QTY TEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIR COND &amp; PRESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK(S) SET, BLEEDS ON, SET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTRUMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X-CHECKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RADIOS, RADAR, TRANSPONDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OXYGEN &amp; INTERPHONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N1 &amp; IAS BUGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRELIMINARY FLIGHT COMPARTMENT CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OVERHEAT DETECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLEARED FOR START PROCEDURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIRE WARNING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISOLATION VLV OPEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTINGUISHER TEST SWITCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HYDRAULIC PANEL SET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARGO SMOKE/FIRE SYSTEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APU (IF REQUIRED)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START/ON BUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VERIFY TAKEOFF SPEEDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANNOUNCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMERGENCY EQUIPMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIRCUIT BREAKERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLIGHT RECORDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLEARED FOR START CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOBILE PHONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START PRESSURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASSENGER OXYGEN SWITCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTICOLLISION LIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GALLEY POWER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOORS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIR CONDITIONING PACKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO SMOKING SIGNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTO PILOT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISENGAGED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTI-SKID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLAP LEVER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STABILIZER TRIM CUTOUT SWITCHES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHEEL WELL FIRE WARNING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIGHT TEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FREE &amp; ZERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAVIGATION TRANSFER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAPERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ON BOARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMC/CDU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCENT APPROACH CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTI–ICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTIMETER &amp; INSTRUMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET &amp; X-CHECKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFTER START PROCEDURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFTER START CHECKLIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELECTRICAL GENERATORS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACKS ON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLIGHT CONTROLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CABIN DOOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LANDING LIGHTS &amp; STROBES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS/IAS or HDG/IAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELECTRICAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ON GPU/APU</t>
   </si>
   <si>
     <t xml:space="preserve">FASTEN BELTS</t>
@@ -1240,7 +1287,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1323,6 +1370,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1696,15 +1750,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1791,21 +1845,21 @@
   </sheetPr>
   <dimension ref="A1:L433"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B155" activeCellId="0" sqref="B155:B157"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G135" activeCellId="0" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,7 +2260,7 @@
       <c r="A36" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
         <v>84</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -2887,7 +2941,7 @@
       <c r="K76" s="19"/>
       <c r="L76" s="19"/>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D77" s="9" t="s">
         <v>178</v>
       </c>
@@ -2900,7 +2954,7 @@
       <c r="K77" s="19"/>
       <c r="L77" s="19"/>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D78" s="9" t="s">
         <v>180</v>
       </c>
@@ -2913,11 +2967,11 @@
       <c r="K78" s="19"/>
       <c r="L78" s="19"/>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="9" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E79" s="33" t="s">
         <v>183</v>
       </c>
       <c r="H79" s="19"/>
@@ -2926,13 +2980,9 @@
       <c r="K79" s="19"/>
       <c r="L79" s="19"/>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>185</v>
-      </c>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D80" s="0"/>
+      <c r="E80" s="0"/>
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
@@ -2953,7 +3003,7 @@
       <c r="K81" s="19"/>
       <c r="L81" s="19"/>
     </row>
-    <row r="82" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="7.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="D82" s="19"/>
@@ -2966,11 +3016,11 @@
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B83" s="34"/>
       <c r="D83" s="24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E83" s="25"/>
       <c r="H83" s="19"/>
@@ -2981,13 +3031,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>16</v>
@@ -2998,18 +3048,18 @@
       <c r="K84" s="19"/>
       <c r="L84" s="19"/>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>190</v>
+        <v>128</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>165</v>
+        <v>22</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E85" s="35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
@@ -3017,12 +3067,12 @@
       <c r="K85" s="19"/>
       <c r="L85" s="19"/>
     </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="D86" s="19"/>
       <c r="E86" s="19"/>
@@ -3032,15 +3082,15 @@
       <c r="K86" s="19"/>
       <c r="L86" s="19"/>
     </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D87" s="34" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E87" s="34"/>
       <c r="H87" s="19"/>
@@ -3049,15 +3099,15 @@
       <c r="K87" s="19"/>
       <c r="L87" s="19"/>
     </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E88" s="18" t="s">
         <v>16</v>
@@ -3068,18 +3118,18 @@
       <c r="K88" s="19"/>
       <c r="L88" s="19"/>
     </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>16</v>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
@@ -3087,12 +3137,18 @@
       <c r="K89" s="19"/>
       <c r="L89" s="19"/>
     </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="D90" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
@@ -3100,16 +3156,12 @@
       <c r="K90" s="19"/>
       <c r="L90" s="19"/>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="B91" s="25"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D91" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
@@ -3117,13 +3169,11 @@
       <c r="K91" s="19"/>
       <c r="L91" s="19"/>
     </row>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="B92" s="27" t="s">
-        <v>22</v>
-      </c>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" s="25"/>
       <c r="D92" s="9" t="s">
         <v>83</v>
       </c>
@@ -3136,18 +3186,18 @@
       <c r="K92" s="19"/>
       <c r="L92" s="19"/>
     </row>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="26" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
@@ -3155,78 +3205,78 @@
       <c r="K93" s="19"/>
       <c r="L93" s="19"/>
     </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="26" t="s">
-        <v>210</v>
+        <v>128</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E94" s="33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="26" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="19"/>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="B96" s="28" t="s">
-        <v>212</v>
+        <v>115</v>
+      </c>
+      <c r="B96" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D97" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="E97" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="B97" s="28" t="s">
+      <c r="B98" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="26" t="s">
+      <c r="D98" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E98" s="27" t="s">
         <v>217</v>
-      </c>
-      <c r="E97" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B98" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="E98" s="27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>216</v>
+        <v>124</v>
+      </c>
+      <c r="B99" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="D99" s="26" t="s">
         <v>83</v>
@@ -3237,69 +3287,69 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="B100" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="D100" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="D100" s="26" t="s">
+      <c r="E100" s="36" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D101" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="E100" s="36" t="s">
+      <c r="E101" s="37" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="29" t="s">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="B101" s="35" t="s">
+      <c r="B102" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="D101" s="29" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0"/>
+      <c r="B103" s="0"/>
+      <c r="D103" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="E101" s="37" t="s">
+      <c r="E103" s="34"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="24" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0"/>
-      <c r="B102" s="0"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24" t="s">
+      <c r="B104" s="25"/>
+      <c r="D104" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B103" s="25"/>
-      <c r="D103" s="34" t="s">
+      <c r="E104" s="17" t="s">
         <v>228</v>
-      </c>
-      <c r="E103" s="34"/>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="B104" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="26" t="s">
-        <v>104</v>
+        <v>221</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E105" s="17" t="s">
         <v>129</v>
@@ -3307,10 +3357,10 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="26" t="s">
-        <v>234</v>
+        <v>104</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D106" s="13" t="s">
         <v>99</v>
@@ -3319,93 +3369,93 @@
         <v>129</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="B107" s="35" t="s">
-        <v>218</v>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0"/>
-      <c r="B108" s="0"/>
+      <c r="A108" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B108" s="35" t="s">
+        <v>214</v>
+      </c>
       <c r="D108" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="E108" s="34"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0"/>
+      <c r="B109" s="0"/>
+      <c r="D109" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E109" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="E108" s="34"/>
-    </row>
-    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="34" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="B109" s="34"/>
-      <c r="D109" s="9" t="s">
+      <c r="B110" s="34"/>
+      <c r="D110" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="E109" s="18" t="s">
+      <c r="E110" s="18" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="9" t="s">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="B110" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="E110" s="18" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="B111" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D111" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="E111" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="9" t="s">
+      <c r="B113" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="B112" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E112" s="18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="B113" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="E113" s="18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="9" t="s">
-        <v>248</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>22</v>
@@ -3419,10 +3469,10 @@
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>250</v>
+        <v>22</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>240</v>
@@ -3432,61 +3482,61 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>219</v>
+      <c r="A116" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B116" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E116" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="19"/>
-      <c r="B117" s="21"/>
+      <c r="A117" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>217</v>
+      </c>
       <c r="D117" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E117" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="B118" s="34"/>
+      <c r="A118" s="19"/>
+      <c r="B118" s="21"/>
       <c r="D118" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E118" s="18" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="B119" s="18" t="s">
+      <c r="A119" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="B119" s="34"/>
+      <c r="D119" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E119" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B120" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="E119" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>22</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>240</v>
@@ -3497,21 +3547,21 @@
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B121" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B122" s="18" t="s">
         <v>22</v>
@@ -3520,26 +3570,26 @@
       <c r="E122" s="19"/>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="16" t="s">
-        <v>260</v>
+      <c r="A123" s="9" t="s">
+        <v>257</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>261</v>
+        <v>22</v>
       </c>
       <c r="D123" s="38" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E123" s="39"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E124" s="18" t="s">
         <v>129</v>
@@ -3547,13 +3597,13 @@
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B125" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E125" s="40" t="s">
         <v>63</v>
@@ -3561,10 +3611,10 @@
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>112</v>
@@ -3575,7 +3625,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B127" s="18" t="s">
         <v>129</v>
@@ -3612,18 +3662,18 @@
         <v>153</v>
       </c>
       <c r="E129" s="18" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E130" s="18" t="s">
         <v>129</v>
@@ -3631,13 +3681,13 @@
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="13" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E131" s="18" t="s">
         <v>129</v>
@@ -3653,11 +3703,11 @@
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="24" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B133" s="25"/>
       <c r="D133" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E133" s="18" t="s">
         <v>22</v>
@@ -3665,7 +3715,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="26" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B134" s="27" t="s">
         <v>22</v>
@@ -3680,7 +3730,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="26" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B135" s="27" t="s">
         <v>165</v>
@@ -3695,13 +3745,13 @@
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B136" s="27" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E136" s="18" t="s">
         <v>76</v>
@@ -3709,13 +3759,13 @@
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B137" s="27" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E137" s="14" t="s">
         <v>76</v>
@@ -3723,21 +3773,21 @@
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B138" s="35" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D139" s="41" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E139" s="42"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B140" s="5"/>
       <c r="D140" s="26" t="s">
@@ -3749,7 +3799,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B141" s="18"/>
       <c r="D141" s="26" t="s">
@@ -3761,7 +3811,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B142" s="18"/>
       <c r="D142" s="26" t="s">
@@ -3777,15 +3827,15 @@
       </c>
       <c r="B143" s="18"/>
       <c r="D143" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E143" s="28" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B144" s="18"/>
       <c r="D144" s="26" t="s">
@@ -3797,7 +3847,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B145" s="18"/>
       <c r="D145" s="26" t="s">
@@ -3809,11 +3859,11 @@
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B146" s="18"/>
       <c r="D146" s="29" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E146" s="35" t="s">
         <v>129</v>
@@ -3821,27 +3871,27 @@
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B147" s="18"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B148" s="18"/>
       <c r="D148" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E148" s="5"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B149" s="18"/>
       <c r="D149" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E149" s="18" t="s">
         <v>129</v>
@@ -3849,11 +3899,11 @@
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B150" s="18"/>
       <c r="D150" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E150" s="18" t="s">
         <v>129</v>
@@ -3861,11 +3911,11 @@
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B151" s="18"/>
       <c r="D151" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E151" s="18" t="s">
         <v>129</v>
@@ -3873,11 +3923,11 @@
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="13" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B152" s="14"/>
       <c r="D152" s="9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E152" s="18" t="s">
         <v>129</v>
@@ -3885,7 +3935,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D153" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E153" s="18" t="s">
         <v>129</v>
@@ -3893,13 +3943,13 @@
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="24" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E154" s="18" t="s">
         <v>129</v>
@@ -3907,13 +3957,13 @@
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="26" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E155" s="18" t="s">
         <v>129</v>
@@ -3921,13 +3971,13 @@
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B156" s="27" t="s">
         <v>216</v>
       </c>
       <c r="D156" s="13" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E156" s="14" t="s">
         <v>129</v>
@@ -3938,32 +3988,32 @@
         <v>124</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="26" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B158" s="28" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="26" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B159" s="28" t="s">
         <v>143</v>
       </c>
       <c r="D159" s="26" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E159" s="28" t="s">
         <v>129</v>
@@ -3971,21 +4021,23 @@
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="29" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B160" s="35" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D160" s="26" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E160" s="28" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0"/>
+      <c r="B161" s="0"/>
       <c r="D161" s="26" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E161" s="28" t="s">
         <v>129</v>
@@ -3993,7 +4045,7 @@
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D162" s="29" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E162" s="35" t="s">
         <v>129</v>
@@ -4252,8 +4304,8 @@
     <mergeCell ref="D87:E87"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="D108:E108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A119:B119"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4273,25 +4325,25 @@
   <dimension ref="A1:L433"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D172" activeCellId="1" sqref="B155:B157 D172"/>
+      <selection pane="topLeft" activeCell="D172" activeCellId="0" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4328,7 +4380,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="10"/>
@@ -4391,7 +4443,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>63</v>
@@ -4407,7 +4459,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
@@ -4697,7 +4749,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>22</v>
@@ -4777,13 +4829,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>22</v>
@@ -4799,10 +4851,10 @@
         <v>16</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
@@ -4813,16 +4865,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
@@ -4839,10 +4891,10 @@
         <v>76</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
@@ -4896,7 +4948,7 @@
         <v>16</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>16</v>
@@ -4934,7 +4986,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E51" s="28" t="s">
         <v>216</v>
@@ -4966,7 +5018,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D53" s="29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E53" s="35" t="s">
         <v>16</v>
@@ -4979,7 +5031,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="24" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B54" s="25"/>
       <c r="H54" s="19"/>
@@ -4990,13 +5042,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B55" s="28" t="s">
         <v>216</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E55" s="15"/>
       <c r="H55" s="19"/>
@@ -5007,13 +5059,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>216</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>116</v>
@@ -5026,13 +5078,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="26" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>216</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>16</v>
@@ -5045,7 +5097,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="26" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>216</v>
@@ -5064,16 +5116,16 @@
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="26" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H59" s="19"/>
       <c r="I59" s="19"/>
@@ -5083,7 +5135,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B60" s="28" t="s">
         <v>216</v>
@@ -5102,7 +5154,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="26" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>216</v>
@@ -5115,13 +5167,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="26" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E62" s="25"/>
       <c r="H62" s="19"/>
@@ -5135,10 +5187,10 @@
         <v>142</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>129</v>
@@ -5154,10 +5206,10 @@
         <v>59</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E64" s="28" t="s">
         <v>16</v>
@@ -5170,13 +5222,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="26" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E65" s="27" t="s">
         <v>22</v>
@@ -5189,16 +5241,16 @@
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>22</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
@@ -5214,7 +5266,7 @@
         <v>93</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E67" s="35" t="s">
         <v>129</v>
@@ -5227,7 +5279,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="26" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>16</v>
@@ -5240,10 +5292,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="26" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>156</v>
@@ -5257,7 +5309,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="26" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>22</v>
@@ -5270,7 +5322,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="26" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>216</v>
@@ -5289,10 +5341,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>162</v>
@@ -5308,7 +5360,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="26" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B73" s="28" t="s">
         <v>216</v>
@@ -5327,7 +5379,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="26" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B74" s="28" t="s">
         <v>216</v>
@@ -5349,7 +5401,7 @@
         <v>107</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>166</v>
@@ -5384,10 +5436,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="26" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="H77" s="19"/>
       <c r="I77" s="20"/>
@@ -5397,10 +5449,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="26" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="20"/>
@@ -5410,7 +5462,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="29" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B79" s="35" t="s">
         <v>16</v>
@@ -5430,7 +5482,7 @@
     </row>
     <row r="81" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5459,10 +5511,10 @@
       </c>
       <c r="B83" s="5"/>
       <c r="D83" s="24" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
@@ -5472,13 +5524,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>178</v>
+        <v>369</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>179</v>
+        <v>370</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>57</v>
@@ -5491,13 +5543,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>180</v>
+        <v>372</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>181</v>
+        <v>373</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E85" s="28" t="s">
         <v>16</v>
@@ -5510,16 +5562,16 @@
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E86" s="28" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
@@ -5529,10 +5581,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B87" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>374</v>
@@ -5548,7 +5600,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D88" s="26" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E88" s="28" t="s">
         <v>216</v>
@@ -5578,13 +5630,13 @@
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E90" s="35" t="s">
         <v>143</v>
@@ -5610,13 +5662,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D92" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D92" s="34" t="s">
-        <v>197</v>
       </c>
       <c r="E92" s="34"/>
       <c r="H92" s="19"/>
@@ -5627,13 +5679,13 @@
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>129</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E93" s="18" t="s">
         <v>16</v>
@@ -5652,18 +5704,18 @@
         <v>16</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D95" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5672,10 +5724,10 @@
       </c>
       <c r="B96" s="25"/>
       <c r="D96" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5700,21 +5752,21 @@
         <v>22</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>57</v>
       </c>
       <c r="D99" s="45" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>16</v>
@@ -5722,7 +5774,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>379</v>
@@ -5736,29 +5788,29 @@
         <v>165</v>
       </c>
       <c r="D101" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>57</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E102" s="28" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B103" s="30" t="s">
         <v>212</v>
@@ -5772,27 +5824,27 @@
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D104" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E104" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B105" s="25"/>
       <c r="D105" s="29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E105" s="35" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B106" s="28" t="s">
         <v>216</v>
@@ -5806,22 +5858,22 @@
         <v>216</v>
       </c>
       <c r="D107" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E107" s="34"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B108" s="27" t="s">
         <v>229</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E108" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5829,24 +5881,24 @@
         <v>104</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E110" s="18" t="s">
         <v>129</v>
@@ -5860,18 +5912,18 @@
         <v>136</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E111" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D112" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E112" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5902,13 +5954,13 @@
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E115" s="18" t="s">
         <v>22</v>
@@ -5916,13 +5968,13 @@
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B116" s="18" t="s">
         <v>129</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E116" s="18" t="s">
         <v>129</v>
@@ -5930,7 +5982,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B117" s="18" t="s">
         <v>22</v>
@@ -5944,39 +5996,39 @@
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D120" s="38" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E120" s="39"/>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="34" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B121" s="34"/>
       <c r="D121" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E121" s="18" t="s">
         <v>129</v>
@@ -5984,13 +6036,13 @@
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B122" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E122" s="40" t="s">
         <v>63</v>
@@ -5998,7 +6050,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B123" s="18" t="s">
         <v>22</v>
@@ -6012,7 +6064,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B124" s="18" t="s">
         <v>22</v>
@@ -6026,10 +6078,10 @@
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>34</v>
@@ -6040,10 +6092,10 @@
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="16" t="s">
-        <v>263</v>
+        <v>383</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>98</v>
@@ -6054,13 +6106,13 @@
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B127" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E127" s="18" t="s">
         <v>129</v>
@@ -6068,13 +6120,13 @@
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E128" s="18" t="s">
         <v>129</v>
@@ -6082,7 +6134,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B129" s="18" t="s">
         <v>129</v>
@@ -6102,7 +6154,7 @@
         <v>129</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E130" s="18" t="s">
         <v>22</v>
@@ -6124,10 +6176,10 @@
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>138</v>
@@ -6138,13 +6190,13 @@
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="13" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E133" s="18" t="s">
         <v>76</v>
@@ -6152,7 +6204,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D134" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E134" s="14" t="s">
         <v>76</v>
@@ -6161,26 +6213,26 @@
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="24" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B135" s="25"/>
       <c r="F135" s="19"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="26" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B136" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D136" s="41" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E136" s="42"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="26" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B137" s="27" t="s">
         <v>22</v>
@@ -6194,13 +6246,13 @@
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B138" s="27" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E138" s="28" t="s">
         <v>57</v>
@@ -6208,27 +6260,27 @@
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B139" s="27" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D139" s="26" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E139" s="28" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B140" s="35" t="s">
-        <v>282</v>
+        <v>387</v>
       </c>
       <c r="D140" s="26" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E140" s="28" t="s">
         <v>129</v>
@@ -6244,7 +6296,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B142" s="5"/>
       <c r="D142" s="26" t="s">
@@ -6256,11 +6308,11 @@
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B143" s="18"/>
       <c r="D143" s="26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E143" s="28" t="s">
         <v>129</v>
@@ -6268,7 +6320,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B144" s="18"/>
       <c r="D144" s="26" t="s">
@@ -6292,23 +6344,23 @@
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B146" s="18"/>
       <c r="D146" s="26" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E146" s="28" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B147" s="18"/>
       <c r="D147" s="26" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E147" s="28" t="s">
         <v>57</v>
@@ -6316,11 +6368,11 @@
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B148" s="18"/>
       <c r="D148" s="26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E148" s="28" t="s">
         <v>129</v>
@@ -6328,11 +6380,11 @@
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B149" s="18"/>
       <c r="D149" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E149" s="28" t="s">
         <v>129</v>
@@ -6340,7 +6392,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B150" s="18"/>
       <c r="D150" s="26" t="s">
@@ -6352,11 +6404,11 @@
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B151" s="18"/>
       <c r="D151" s="26" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E151" s="28" t="s">
         <v>84</v>
@@ -6364,19 +6416,19 @@
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B152" s="18"/>
       <c r="D152" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E152" s="28" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B153" s="18"/>
       <c r="D153" s="26" t="s">
@@ -6388,11 +6440,11 @@
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="13" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B154" s="14"/>
       <c r="D154" s="26" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E154" s="28" t="s">
         <v>19</v>
@@ -6400,7 +6452,7 @@
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D155" s="26" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E155" s="28" t="s">
         <v>129</v>
@@ -6408,10 +6460,10 @@
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D156" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E156" s="35" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6421,7 +6473,7 @@
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -6431,13 +6483,13 @@
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B164" s="5"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B165" s="18" t="s">
         <v>129</v>
@@ -6445,7 +6497,7 @@
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B166" s="18" t="s">
         <v>129</v>
@@ -6453,7 +6505,7 @@
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B167" s="18" t="s">
         <v>129</v>
@@ -6461,7 +6513,7 @@
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B168" s="18" t="s">
         <v>129</v>
@@ -6469,7 +6521,7 @@
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B169" s="18" t="s">
         <v>129</v>
@@ -6477,7 +6529,7 @@
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B170" s="18" t="s">
         <v>129</v>
@@ -6485,7 +6537,7 @@
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B171" s="18" t="s">
         <v>129</v>
@@ -6493,7 +6545,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="13" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B172" s="14" t="s">
         <v>129</v>
@@ -6502,15 +6554,15 @@
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="4" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="26" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B175" s="28" t="s">
         <v>129</v>
@@ -6518,7 +6570,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="26" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B176" s="28" t="s">
         <v>129</v>
@@ -6526,7 +6578,7 @@
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="26" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B177" s="28" t="s">
         <v>129</v>
@@ -6534,15 +6586,15 @@
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="26" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B178" s="28" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="29" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B179" s="35" t="s">
         <v>129</v>

</xml_diff>